<commit_message>
I edited window "Europa"
</commit_message>
<xml_diff>
--- a/Europe_book.xlsx
+++ b/Europe_book.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,79 +424,44 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Країна</t>
+          <t>Інформація по Азії</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>81,532,629</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Останнє оновлення</t>
+          <t>Всього випадків</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021-11-21 00:00:00</t>
+          <t>1,204,513</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Усього випадків</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1581500</v>
+          <t>Загальна кількість смертей</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>78,786,289</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Невідома</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>50.8333</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Невідома</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4.469936</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
           <t>Число одуживших</t>
         </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Смертність</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>26568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>